<commit_message>
add: add 1-3 files
</commit_message>
<xml_diff>
--- a/整理数据.xlsx
+++ b/整理数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyouyu/WorkSpace/Lab106/Lab_Data/BMG_Data_SHU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yuyouyu\SHU\BMG_Data_SHU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030BA25-65B0-D640-863A-C151B84F9F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED8ECE8-C9B9-483E-B0D7-7A1F5A53DD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -100,15 +91,6 @@
   </si>
   <si>
     <t>[19]</t>
-  </si>
-  <si>
-    <t>Zr52.5Al10Ti5Cu17.9Ni14.6</t>
-  </si>
-  <si>
-    <t>Zr61Cu17.5Ni10Al7.5Si4</t>
-  </si>
-  <si>
-    <t>Zr57Nb5Cu15.4Ni12.6Al10</t>
   </si>
   <si>
     <t>Zr57Cu18.67Ni8Al16.33</t>
@@ -885,12 +867,24 @@
   <si>
     <t>[41, 42]</t>
   </si>
+  <si>
+    <t>Zr52.5Al10Ti5Cu17.9Ni14.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zr61Cu17.5Ni10Al7.5Si4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zr57Nb5Cu15.4Ni12.6Al10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -979,7 +973,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1023,6 +1017,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1341,33 +1338,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1966D2F-1FA9-5C45-AC98-B0EB4D799C65}">
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" activeCellId="1" sqref="C77 B57"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
@@ -1382,20 +1379,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3">
+        <v>259</v>
+      </c>
+      <c r="B2" s="19">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="19">
         <v>665</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="19">
         <v>723</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="19">
         <v>1090</v>
       </c>
       <c r="F2" s="3">
@@ -1411,9 +1408,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>260</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1428,9 +1425,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>261</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -1455,9 +1452,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
@@ -1480,9 +1477,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -1505,9 +1502,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
@@ -1530,9 +1527,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -1555,9 +1552,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>12</v>
@@ -1582,9 +1579,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3">
         <v>12</v>
@@ -1609,9 +1606,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3">
         <v>12</v>
@@ -1636,9 +1633,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3">
         <v>12</v>
@@ -1663,9 +1660,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
@@ -1690,9 +1687,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3">
         <v>12</v>
@@ -1717,9 +1714,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3">
         <v>8</v>
@@ -1744,9 +1741,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>8</v>
@@ -1771,9 +1768,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>8</v>
@@ -1798,9 +1795,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -1825,9 +1822,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3">
         <v>8</v>
@@ -1852,9 +1849,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>8</v>
@@ -1879,9 +1876,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3">
         <v>8</v>
@@ -1906,9 +1903,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3">
         <v>8</v>
@@ -1933,9 +1930,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3">
         <v>8</v>
@@ -1962,9 +1959,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="3">
         <v>8</v>
@@ -1991,9 +1988,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3">
         <v>8</v>
@@ -2020,9 +2017,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26" s="3">
         <v>8</v>
@@ -2049,9 +2046,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
@@ -2076,9 +2073,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B28" s="3">
         <v>2</v>
@@ -2103,9 +2100,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
@@ -2130,9 +2127,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B30" s="3">
         <v>8</v>
@@ -2159,9 +2156,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31" s="3">
         <v>8</v>
@@ -2188,9 +2185,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3">
         <v>8</v>
@@ -2217,9 +2214,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="3">
         <v>8</v>
@@ -2246,9 +2243,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B34" s="3">
         <v>3</v>
@@ -2271,9 +2268,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3">
         <v>3</v>
@@ -2296,9 +2293,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B36" s="3">
         <v>3</v>
@@ -2321,9 +2318,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B37" s="3">
         <v>5</v>
@@ -2344,9 +2341,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B38" s="3">
         <v>15</v>
@@ -2371,9 +2368,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B39" s="3">
         <v>12</v>
@@ -2398,9 +2395,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B40" s="3">
         <v>8</v>
@@ -2421,9 +2418,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B41" s="3">
         <v>15</v>
@@ -2444,9 +2441,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B42" s="3">
         <v>12</v>
@@ -2465,9 +2462,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B43" s="3">
         <v>18</v>
@@ -2486,9 +2483,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B44" s="3">
         <v>10</v>
@@ -2515,9 +2512,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B45" s="3">
         <v>3</v>
@@ -2540,9 +2537,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B46" s="3">
         <v>4</v>
@@ -2565,9 +2562,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B47" s="3">
         <v>4</v>
@@ -2590,9 +2587,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3">
         <v>4</v>
@@ -2615,9 +2612,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3">
         <v>3</v>
@@ -2638,9 +2635,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -2665,9 +2662,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B51" s="3">
         <v>2</v>
@@ -2692,9 +2689,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -2719,9 +2716,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" s="3">
         <v>2</v>
@@ -2746,9 +2743,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B54" s="3">
         <v>2</v>
@@ -2773,9 +2770,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="18" customFormat="1">
+    <row r="55" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B55" s="14">
         <v>73</v>
@@ -2795,12 +2792,12 @@
       </c>
       <c r="H55" s="16"/>
       <c r="I55" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B56" s="9">
         <v>12.6</v>
@@ -2820,12 +2817,12 @@
         <v>3.5</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B57" s="9">
         <v>16</v>
@@ -2847,12 +2844,12 @@
       </c>
       <c r="H57" s="11"/>
       <c r="I57" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B58" s="9">
         <v>4</v>
@@ -2872,12 +2869,12 @@
       <c r="G58" s="10"/>
       <c r="H58" s="11"/>
       <c r="I58" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B59" s="9">
         <v>4</v>
@@ -2895,12 +2892,12 @@
       <c r="G59" s="10"/>
       <c r="H59" s="11"/>
       <c r="I59" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B60" s="9">
         <v>4</v>
@@ -2918,12 +2915,12 @@
       <c r="G60" s="10"/>
       <c r="H60" s="11"/>
       <c r="I60" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B61" s="9">
         <v>4</v>
@@ -2941,12 +2938,12 @@
       <c r="G61" s="10"/>
       <c r="H61" s="9"/>
       <c r="I61" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="8" t="s">
-        <v>236</v>
       </c>
       <c r="B62" s="9">
         <v>4</v>
@@ -2964,12 +2961,12 @@
       <c r="G62" s="10"/>
       <c r="H62" s="11"/>
       <c r="I62" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B63" s="9">
         <v>4</v>
@@ -2987,12 +2984,12 @@
       <c r="G63" s="10"/>
       <c r="H63" s="11"/>
       <c r="I63" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B64" s="9">
         <v>4</v>
@@ -3010,12 +3007,12 @@
       <c r="G64" s="10"/>
       <c r="H64" s="11"/>
       <c r="I64" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B65" s="9">
         <v>4</v>
@@ -3033,12 +3030,12 @@
       <c r="G65" s="10"/>
       <c r="H65" s="11"/>
       <c r="I65" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B66" s="9">
         <v>6</v>
@@ -3060,12 +3057,12 @@
         <v>14.5</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B67" s="9">
         <v>10</v>
@@ -3083,12 +3080,12 @@
       <c r="G67" s="10"/>
       <c r="H67" s="11"/>
       <c r="I67" s="12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B68" s="9">
         <v>14</v>
@@ -3108,12 +3105,12 @@
       </c>
       <c r="H68" s="11"/>
       <c r="I68" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B69" s="9">
         <v>6</v>
@@ -3135,12 +3132,12 @@
         <v>0</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B70" s="9">
         <v>10</v>
@@ -3162,12 +3159,12 @@
         <v>0</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B71" s="9">
         <v>14</v>
@@ -3185,12 +3182,12 @@
       <c r="G71" s="10"/>
       <c r="H71" s="9"/>
       <c r="I71" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B72" s="9">
         <v>14</v>
@@ -3208,12 +3205,12 @@
       <c r="G72" s="10"/>
       <c r="H72" s="11"/>
       <c r="I72" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B73" s="9">
         <v>18</v>
@@ -3235,12 +3232,12 @@
         <v>3.5</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B74" s="9">
         <v>3</v>
@@ -3262,12 +3259,12 @@
         <v>0</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B75" s="9">
         <v>3</v>
@@ -3287,12 +3284,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B76" s="9">
         <v>4</v>
@@ -3314,12 +3311,12 @@
         <v>2.5</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B77" s="9">
         <v>2</v>
@@ -3339,12 +3336,12 @@
         <v>0</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" s="1" customFormat="1">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B78" s="4">
         <v>14</v>
@@ -3362,12 +3359,12 @@
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B79" s="3">
         <v>8</v>
@@ -3385,12 +3382,12 @@
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B80" s="3">
         <v>2.5</v>
@@ -3408,12 +3405,12 @@
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -3427,12 +3424,12 @@
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3">
@@ -3448,12 +3445,12 @@
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -3467,12 +3464,12 @@
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -3486,12 +3483,12 @@
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3">
@@ -3507,12 +3504,12 @@
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="5">
@@ -3532,12 +3529,12 @@
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="5">
@@ -3555,12 +3552,12 @@
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="5">
@@ -3578,12 +3575,12 @@
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="5">
@@ -3601,13 +3598,13 @@
       <c r="G89" s="5"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="5">
@@ -3625,12 +3622,12 @@
       <c r="G90" s="5"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="5">
@@ -3648,12 +3645,12 @@
       <c r="G91" s="5"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="5">
@@ -3669,12 +3666,12 @@
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="5">
@@ -3692,12 +3689,12 @@
       <c r="G93" s="5"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="5">
@@ -3713,12 +3710,12 @@
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="5">
@@ -3736,12 +3733,12 @@
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="5">
@@ -3757,12 +3754,12 @@
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="5">
@@ -3782,12 +3779,12 @@
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="5">
@@ -3807,35 +3804,35 @@
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F99" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="5">
@@ -3853,12 +3850,12 @@
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="5">
@@ -3876,12 +3873,12 @@
       <c r="G101" s="5"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="5"/>
@@ -3889,16 +3886,16 @@
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="5">
@@ -3916,12 +3913,12 @@
       <c r="G103" s="5"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="5">
@@ -3939,12 +3936,12 @@
       <c r="G104" s="5"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="5">
@@ -3964,12 +3961,12 @@
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="5">
@@ -3989,12 +3986,12 @@
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="5">
@@ -4012,12 +4009,12 @@
       <c r="G107" s="5"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="5">
@@ -4033,12 +4030,12 @@
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="5">
@@ -4058,12 +4055,12 @@
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="5"/>
@@ -4075,12 +4072,12 @@
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="5">
@@ -4096,12 +4093,12 @@
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="5">
@@ -4119,12 +4116,12 @@
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -4136,12 +4133,12 @@
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -4153,12 +4150,12 @@
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B115" s="5"/>
       <c r="C115" s="5">
@@ -4174,12 +4171,12 @@
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B116" s="5"/>
       <c r="C116" s="5">
@@ -4195,12 +4192,12 @@
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
@@ -4212,12 +4209,12 @@
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="5">
@@ -4233,12 +4230,12 @@
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="5">
@@ -4254,12 +4251,12 @@
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -4271,12 +4268,12 @@
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
@@ -4288,12 +4285,12 @@
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B122" s="5"/>
       <c r="C122" s="5">
@@ -4309,12 +4306,12 @@
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B123" s="5"/>
       <c r="C123" s="5">
@@ -4332,12 +4329,12 @@
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="5">
@@ -4353,12 +4350,12 @@
       <c r="G124" s="5"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
@@ -4370,12 +4367,12 @@
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B126" s="5"/>
       <c r="C126" s="5">
@@ -4391,12 +4388,12 @@
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
@@ -4408,12 +4405,12 @@
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -4425,12 +4422,12 @@
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -4442,12 +4439,12 @@
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="5">
@@ -4463,12 +4460,12 @@
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B131" s="5"/>
       <c r="C131" s="5">
@@ -4484,12 +4481,12 @@
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B132" s="5"/>
       <c r="C132" s="5">
@@ -4505,12 +4502,12 @@
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B133" s="5"/>
       <c r="C133" s="5">
@@ -4524,12 +4521,12 @@
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
@@ -4541,12 +4538,12 @@
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B135" s="5"/>
       <c r="C135" s="5">
@@ -4562,12 +4559,12 @@
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B136" s="5"/>
       <c r="C136" s="5">
@@ -4583,16 +4580,16 @@
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
@@ -4602,12 +4599,12 @@
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="5">
@@ -4623,12 +4620,12 @@
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -4640,12 +4637,12 @@
       </c>
       <c r="H139" s="3"/>
       <c r="I139" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
@@ -4657,12 +4654,12 @@
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -4674,12 +4671,12 @@
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -4691,12 +4688,12 @@
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -4712,12 +4709,12 @@
       <c r="G143" s="5"/>
       <c r="H143" s="3"/>
       <c r="I143" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="5">
@@ -4733,12 +4730,12 @@
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B145" s="5"/>
       <c r="C145" s="5">
@@ -4754,12 +4751,12 @@
       </c>
       <c r="H145" s="3"/>
       <c r="I145" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B146" s="5"/>
       <c r="C146" s="5">
@@ -4775,12 +4772,12 @@
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -4792,12 +4789,12 @@
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
@@ -4809,12 +4806,12 @@
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B149" s="5"/>
       <c r="C149" s="5">
@@ -4830,12 +4827,12 @@
       </c>
       <c r="H149" s="3"/>
       <c r="I149" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B150" s="5"/>
       <c r="C150" s="5">
@@ -4851,12 +4848,12 @@
       </c>
       <c r="H150" s="3"/>
       <c r="I150" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B151" s="5"/>
       <c r="C151" s="5">
@@ -4872,12 +4869,12 @@
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B152" s="5"/>
       <c r="C152" s="5">
@@ -4895,12 +4892,12 @@
       </c>
       <c r="H152" s="3"/>
       <c r="I152" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
@@ -4912,12 +4909,12 @@
       </c>
       <c r="H153" s="3"/>
       <c r="I153" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
@@ -4929,12 +4926,12 @@
       </c>
       <c r="H154" s="3"/>
       <c r="I154" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
@@ -4946,12 +4943,12 @@
       </c>
       <c r="H155" s="3"/>
       <c r="I155" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B156" s="5"/>
       <c r="C156" s="5">
@@ -4965,16 +4962,16 @@
       </c>
       <c r="H156" s="3"/>
       <c r="I156" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B157" s="5"/>
       <c r="C157" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
@@ -4984,12 +4981,12 @@
       </c>
       <c r="H157" s="3"/>
       <c r="I157" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
@@ -5001,12 +4998,12 @@
       </c>
       <c r="H158" s="3"/>
       <c r="I158" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
@@ -5018,12 +5015,12 @@
       </c>
       <c r="H159" s="3"/>
       <c r="I159" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B160" s="5"/>
       <c r="C160" s="5">
@@ -5039,12 +5036,12 @@
       </c>
       <c r="H160" s="3"/>
       <c r="I160" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
@@ -5056,12 +5053,12 @@
       </c>
       <c r="H161" s="3"/>
       <c r="I161" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B162" s="5"/>
       <c r="C162" s="5">
@@ -5077,12 +5074,12 @@
       </c>
       <c r="H162" s="3"/>
       <c r="I162" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5">
@@ -5091,57 +5088,57 @@
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G163" s="5">
         <v>112</v>
       </c>
       <c r="H163" s="3"/>
       <c r="I163" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
       <c r="F164" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G164" s="5">
         <v>116.4</v>
       </c>
       <c r="H164" s="3"/>
       <c r="I164" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
       <c r="F165" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G165" s="5">
         <v>114.6</v>
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="5">
@@ -5150,19 +5147,19 @@
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
       <c r="F166" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G166" s="5">
         <v>116.5</v>
       </c>
       <c r="H166" s="3"/>
       <c r="I166" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="5">
@@ -5172,7 +5169,7 @@
         <v>1032</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F167" s="3"/>
       <c r="G167" s="6">
@@ -5180,12 +5177,12 @@
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B168" s="5"/>
       <c r="C168" s="5">
@@ -5201,12 +5198,12 @@
       </c>
       <c r="H168" s="5"/>
       <c r="I168" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
@@ -5218,12 +5215,12 @@
       </c>
       <c r="H169" s="5"/>
       <c r="I169" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
@@ -5235,12 +5232,12 @@
       </c>
       <c r="H170" s="5"/>
       <c r="I170" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B171" s="5"/>
       <c r="C171" s="5">
@@ -5250,7 +5247,7 @@
         <v>1038</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F171" s="3"/>
       <c r="G171" s="6">
@@ -5258,12 +5255,12 @@
       </c>
       <c r="H171" s="5"/>
       <c r="I171" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -5275,12 +5272,12 @@
       </c>
       <c r="H172" s="5"/>
       <c r="I172" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B173" s="5"/>
       <c r="C173" s="5">
@@ -5290,7 +5287,7 @@
         <v>1038</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F173" s="3"/>
       <c r="G173" s="6">
@@ -5298,12 +5295,12 @@
       </c>
       <c r="H173" s="5"/>
       <c r="I173" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="5">
@@ -5319,12 +5316,12 @@
       </c>
       <c r="H174" s="5"/>
       <c r="I174" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -5336,12 +5333,12 @@
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="5">
@@ -5351,7 +5348,7 @@
         <v>1035</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F176" s="3"/>
       <c r="G176" s="6">
@@ -5359,12 +5356,12 @@
       </c>
       <c r="H176" s="5"/>
       <c r="I176" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
@@ -5372,16 +5369,16 @@
       <c r="E177" s="5"/>
       <c r="F177" s="5"/>
       <c r="G177" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -5389,16 +5386,16 @@
       <c r="E178" s="5"/>
       <c r="F178" s="5"/>
       <c r="G178" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H178" s="5"/>
       <c r="I178" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
@@ -5408,16 +5405,16 @@
         <v>1190</v>
       </c>
       <c r="G179" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H179" s="5"/>
       <c r="I179" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
@@ -5425,16 +5422,16 @@
       <c r="E180" s="5"/>
       <c r="F180" s="5"/>
       <c r="G180" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H180" s="5"/>
       <c r="I180" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -5448,12 +5445,12 @@
       </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B182" s="7"/>
       <c r="C182" s="7">
@@ -5471,12 +5468,12 @@
       </c>
       <c r="H182" s="3"/>
       <c r="I182" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -5490,12 +5487,12 @@
       </c>
       <c r="H183" s="3"/>
       <c r="I183" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -5509,12 +5506,12 @@
       </c>
       <c r="H184" s="3"/>
       <c r="I184" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -5530,12 +5527,12 @@
       </c>
       <c r="H185" s="3"/>
       <c r="I185" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -5549,12 +5546,12 @@
       </c>
       <c r="H186" s="3"/>
       <c r="I186" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B187" s="3"/>
       <c r="C187" s="5">
@@ -5572,12 +5569,12 @@
       </c>
       <c r="H187" s="3"/>
       <c r="I187" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B188" s="3"/>
       <c r="C188" s="5">
@@ -5595,12 +5592,12 @@
       </c>
       <c r="H188" s="3"/>
       <c r="I188" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B189" s="3"/>
       <c r="C189" s="5">
@@ -5618,12 +5615,12 @@
       </c>
       <c r="H189" s="3"/>
       <c r="I189" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B190" s="3"/>
       <c r="C190" s="5"/>
@@ -5639,12 +5636,12 @@
       </c>
       <c r="H190" s="3"/>
       <c r="I190" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B191" s="3"/>
       <c r="C191" s="5">
@@ -5662,12 +5659,12 @@
       </c>
       <c r="H191" s="3"/>
       <c r="I191" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B192" s="3"/>
       <c r="C192" s="5"/>
@@ -5683,12 +5680,12 @@
       </c>
       <c r="H192" s="3"/>
       <c r="I192" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B193" s="3"/>
       <c r="C193" s="5"/>
@@ -5704,12 +5701,12 @@
       </c>
       <c r="H193" s="3"/>
       <c r="I193" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B194" s="3"/>
       <c r="C194" s="5"/>
@@ -5725,12 +5722,12 @@
       </c>
       <c r="H194" s="3"/>
       <c r="I194" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B195" s="3"/>
       <c r="C195" s="5"/>
@@ -5746,12 +5743,12 @@
       </c>
       <c r="H195" s="3"/>
       <c r="I195" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B196" s="3"/>
       <c r="C196" s="5"/>
@@ -5767,12 +5764,12 @@
       </c>
       <c r="H196" s="3"/>
       <c r="I196" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B197" s="3"/>
       <c r="C197" s="5">
@@ -5790,11 +5787,12 @@
       </c>
       <c r="H197" s="3"/>
       <c r="I197" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: add new 3 file
</commit_message>
<xml_diff>
--- a/整理数据.xlsx
+++ b/整理数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yuyouyu\SHU\BMG_Data_SHU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED8ECE8-C9B9-483E-B0D7-7A1F5A53DD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA7BDAF-A893-4CBD-8934-91F1F1554D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1340,7 +1340,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add: add to 13
</commit_message>
<xml_diff>
--- a/整理数据.xlsx
+++ b/整理数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yuyouyu\SHU\BMG_Data_SHU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyouyu/WorkSpace/Lab106/Lab_Data/BMG_Data_SHU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA7BDAF-A893-4CBD-8934-91F1F1554D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3FC10D-1600-354B-9F4F-4562E2E83FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="271">
   <si>
     <t>σy(MPa)</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>Fe70P12C5Mo5Ni5B2</t>
-  </si>
-  <si>
-    <t>696[2]</t>
   </si>
   <si>
     <t>Fe63P8C7B5Co5Si3Mo2Cr2Al2</t>
@@ -868,15 +865,66 @@
     <t>[41, 42]</t>
   </si>
   <si>
-    <t>Zr52.5Al10Ti5Cu17.9Ni14.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Zr61Cu17.5Ni10Al7.5Si4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Zr57Nb5Cu15.4Ni12.6Al10</t>
+    <t>1600(1200, 1800)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.08(0.02)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>665（675）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>83.4(88.6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zr52.5Al10Ti5Cu17.9Ni14.6(Vit 105)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zr57Nb5Cu15.4Ni12.6Al10(Vit 106)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红色字错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝色字找不到</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>绿色底文献无法找到</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄色底文献中有其他数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>696[2]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,7 +932,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -938,8 +986,56 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -958,6 +1054,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -973,7 +1075,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1020,6 +1122,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1340,19 +1472,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>67</v>
@@ -1379,27 +1513,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2" s="19">
+        <v>263</v>
+      </c>
+      <c r="B2" s="21">
         <v>7</v>
       </c>
-      <c r="C2" s="19">
-        <v>665</v>
-      </c>
-      <c r="D2" s="19">
+      <c r="C2" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="21">
         <v>723</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="3">
         <v>1090</v>
       </c>
       <c r="F2" s="3">
         <v>1654</v>
       </c>
-      <c r="G2" s="3">
-        <v>83.4</v>
+      <c r="G2" s="19" t="s">
+        <v>262</v>
       </c>
       <c r="H2" s="3">
         <v>0.06</v>
@@ -1407,10 +1541,13 @@
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1424,12 +1561,15 @@
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B4" s="3">
+        <v>264</v>
+      </c>
+      <c r="B4" s="21">
         <v>5</v>
       </c>
       <c r="C4" s="3">
@@ -1439,20 +1579,23 @@
       <c r="E4" s="3">
         <v>1115</v>
       </c>
-      <c r="F4" s="3">
-        <v>1600</v>
+      <c r="F4" s="20" t="s">
+        <v>259</v>
       </c>
       <c r="G4" s="3">
         <v>86.7</v>
       </c>
-      <c r="H4" s="3">
-        <v>0.08</v>
+      <c r="H4" s="19" t="s">
+        <v>260</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1476,8 +1619,11 @@
       <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="28" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1527,7 +1673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1552,169 +1698,169 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:10" s="27" customFormat="1">
+      <c r="A9" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="26">
         <v>12</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="26">
         <v>641.6</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="26">
         <v>731.9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="26">
         <v>1168.9000000000001</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="26">
         <v>1872</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26">
         <v>0.1</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:10" s="25" customFormat="1">
+      <c r="A10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C10" s="24">
+        <v>700.4</v>
+      </c>
+      <c r="D10" s="24">
+        <v>786</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1140.8</v>
+      </c>
+      <c r="F10" s="24">
+        <v>1854</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="25" customFormat="1">
+      <c r="A11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="24">
+        <v>699.6</v>
+      </c>
+      <c r="D11" s="24">
+        <v>782</v>
+      </c>
+      <c r="E11" s="24">
+        <v>1138.0999999999999</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1924</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="25" customFormat="1">
+      <c r="A12" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="24">
+        <v>700.3</v>
+      </c>
+      <c r="D12" s="24">
+        <v>781.5</v>
+      </c>
+      <c r="E12" s="24">
+        <v>1134.0999999999999</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1850</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="25" customFormat="1">
+      <c r="A13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" s="24">
+        <v>696.8</v>
+      </c>
+      <c r="D13" s="24">
+        <v>778.6</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1128.2</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1846</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="25" customFormat="1">
+      <c r="A14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="24">
         <v>12</v>
       </c>
-      <c r="C10" s="3">
-        <v>700.4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>786</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1140.8</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1854</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="C14" s="24">
+        <v>698.3</v>
+      </c>
+      <c r="D14" s="24">
+        <v>779.2</v>
+      </c>
+      <c r="E14" s="24">
+        <v>1139</v>
+      </c>
+      <c r="F14" s="24">
+        <v>1874</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3">
-        <v>699.6</v>
-      </c>
-      <c r="D11" s="3">
-        <v>782</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1138.0999999999999</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1924</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3">
-        <v>700.3</v>
-      </c>
-      <c r="D12" s="3">
-        <v>781.5</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1134.0999999999999</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1850</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3">
-        <v>696.8</v>
-      </c>
-      <c r="D13" s="3">
-        <v>778.6</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1128.2</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1846</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3">
-        <v>698.3</v>
-      </c>
-      <c r="D14" s="3">
-        <v>779.2</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1139</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1874</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1740,8 +1886,11 @@
       <c r="I15" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="26">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1768,7 +1917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1795,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1822,7 +1971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1849,7 +1998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1876,7 +2025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1903,7 +2052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -1930,7 +2079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1959,7 +2108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1988,7 +2137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -2017,7 +2166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -2046,7 +2195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -2073,7 +2222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -2100,7 +2249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
@@ -2127,7 +2276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
@@ -2156,7 +2305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
@@ -2185,7 +2334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -2214,7 +2363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
@@ -2243,7 +2392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
@@ -2268,7 +2417,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
@@ -2293,7 +2442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
         <v>53</v>
       </c>
@@ -2318,7 +2467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
         <v>54</v>
       </c>
@@ -2341,9 +2490,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B38" s="3">
         <v>15</v>
@@ -2368,9 +2517,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B39" s="3">
         <v>12</v>
@@ -2395,9 +2544,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B40" s="3">
         <v>8</v>
@@ -2418,7 +2567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="3" t="s">
         <v>55</v>
       </c>
@@ -2441,7 +2590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
@@ -2462,7 +2611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -2483,7 +2632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
@@ -2512,7 +2661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
         <v>59</v>
       </c>
@@ -2537,7 +2686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="3" t="s">
         <v>60</v>
       </c>
@@ -2562,7 +2711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="3" t="s">
         <v>61</v>
       </c>
@@ -2587,7 +2736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
         <v>62</v>
       </c>
@@ -2612,7 +2761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="3" t="s">
         <v>63</v>
       </c>
@@ -2635,9 +2784,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" s="3">
         <v>2</v>
@@ -2662,9 +2811,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" s="3">
         <v>2</v>
@@ -2689,9 +2838,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="3">
         <v>2</v>
@@ -2716,9 +2865,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="3">
         <v>2</v>
@@ -2743,7 +2892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="3" t="s">
         <v>68</v>
       </c>
@@ -2770,9 +2919,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="18" customFormat="1">
       <c r="A55" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B55" s="14">
         <v>73</v>
@@ -2792,12 +2941,12 @@
       </c>
       <c r="H55" s="16"/>
       <c r="I55" s="17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="8" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="B56" s="9">
         <v>12.6</v>
@@ -2817,12 +2966,12 @@
         <v>3.5</v>
       </c>
       <c r="I56" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="8" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="B57" s="9">
         <v>16</v>
@@ -2844,12 +2993,12 @@
       </c>
       <c r="H57" s="11"/>
       <c r="I57" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="8" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="B58" s="9">
         <v>4</v>
@@ -2869,12 +3018,12 @@
       <c r="G58" s="10"/>
       <c r="H58" s="11"/>
       <c r="I58" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="8" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="B59" s="9">
         <v>4</v>
@@ -2892,12 +3041,12 @@
       <c r="G59" s="10"/>
       <c r="H59" s="11"/>
       <c r="I59" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="8" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="B60" s="9">
         <v>4</v>
@@ -2915,12 +3064,12 @@
       <c r="G60" s="10"/>
       <c r="H60" s="11"/>
       <c r="I60" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B61" s="9">
         <v>4</v>
@@ -2938,12 +3087,12 @@
       <c r="G61" s="10"/>
       <c r="H61" s="9"/>
       <c r="I61" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B62" s="9">
         <v>4</v>
@@ -2961,12 +3110,12 @@
       <c r="G62" s="10"/>
       <c r="H62" s="11"/>
       <c r="I62" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B63" s="9">
         <v>4</v>
@@ -2984,12 +3133,12 @@
       <c r="G63" s="10"/>
       <c r="H63" s="11"/>
       <c r="I63" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B64" s="9">
         <v>4</v>
@@ -3007,12 +3156,12 @@
       <c r="G64" s="10"/>
       <c r="H64" s="11"/>
       <c r="I64" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B65" s="9">
         <v>4</v>
@@ -3030,12 +3179,12 @@
       <c r="G65" s="10"/>
       <c r="H65" s="11"/>
       <c r="I65" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B66" s="9">
         <v>6</v>
@@ -3057,12 +3206,12 @@
         <v>14.5</v>
       </c>
       <c r="I66" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="8" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="B67" s="9">
         <v>10</v>
@@ -3080,12 +3229,12 @@
       <c r="G67" s="10"/>
       <c r="H67" s="11"/>
       <c r="I67" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="8" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="B68" s="9">
         <v>14</v>
@@ -3105,12 +3254,12 @@
       </c>
       <c r="H68" s="11"/>
       <c r="I68" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="8" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>243</v>
       </c>
       <c r="B69" s="9">
         <v>6</v>
@@ -3132,12 +3281,12 @@
         <v>0</v>
       </c>
       <c r="I69" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="8" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="B70" s="9">
         <v>10</v>
@@ -3159,12 +3308,12 @@
         <v>0</v>
       </c>
       <c r="I70" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="8" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>247</v>
       </c>
       <c r="B71" s="9">
         <v>14</v>
@@ -3182,12 +3331,12 @@
       <c r="G71" s="10"/>
       <c r="H71" s="9"/>
       <c r="I71" s="12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="8" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="B72" s="9">
         <v>14</v>
@@ -3205,12 +3354,12 @@
       <c r="G72" s="10"/>
       <c r="H72" s="11"/>
       <c r="I72" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B73" s="9">
         <v>18</v>
@@ -3232,12 +3381,12 @@
         <v>3.5</v>
       </c>
       <c r="I73" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="8" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="B74" s="9">
         <v>3</v>
@@ -3259,12 +3408,12 @@
         <v>0</v>
       </c>
       <c r="I74" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="8" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="B75" s="9">
         <v>3</v>
@@ -3284,12 +3433,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B76" s="9">
         <v>4</v>
@@ -3311,12 +3460,12 @@
         <v>2.5</v>
       </c>
       <c r="I76" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="8" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="B77" s="9">
         <v>2</v>
@@ -3336,10 +3485,10 @@
         <v>0</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="1" customFormat="1">
       <c r="A78" s="4" t="s">
         <v>69</v>
       </c>
@@ -3362,7 +3511,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="3" t="s">
         <v>70</v>
       </c>
@@ -3385,7 +3534,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="3" t="s">
         <v>71</v>
       </c>
@@ -3408,7 +3557,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="5" t="s">
         <v>73</v>
       </c>
@@ -3427,7 +3576,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="5" t="s">
         <v>74</v>
       </c>
@@ -3448,7 +3597,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="5" t="s">
         <v>75</v>
       </c>
@@ -3467,7 +3616,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="5" t="s">
         <v>74</v>
       </c>
@@ -3486,7 +3635,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="3" t="s">
         <v>77</v>
       </c>
@@ -3507,7 +3656,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="5" t="s">
         <v>79</v>
       </c>
@@ -3532,7 +3681,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="5" t="s">
         <v>80</v>
       </c>
@@ -3555,7 +3704,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -3578,7 +3727,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -3602,7 +3751,7 @@
       </c>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -3625,7 +3774,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="5" t="s">
         <v>84</v>
       </c>
@@ -3648,7 +3797,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -3669,7 +3818,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="5" t="s">
         <v>86</v>
       </c>
@@ -3692,7 +3841,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="5" t="s">
         <v>87</v>
       </c>
@@ -3713,7 +3862,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="5" t="s">
         <v>88</v>
       </c>
@@ -3736,7 +3885,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="5" t="s">
         <v>89</v>
       </c>
@@ -3757,7 +3906,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9">
       <c r="A97" s="5" t="s">
         <v>90</v>
       </c>
@@ -3782,7 +3931,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9">
       <c r="A98" s="5" t="s">
         <v>91</v>
       </c>
@@ -3807,7 +3956,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" s="5" t="s">
         <v>92</v>
       </c>
@@ -3830,7 +3979,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9">
       <c r="A100" s="5" t="s">
         <v>97</v>
       </c>
@@ -3853,7 +4002,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9">
       <c r="A101" s="5" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +4025,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9">
       <c r="A102" s="5" t="s">
         <v>90</v>
       </c>
@@ -3893,7 +4042,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9">
       <c r="A103" s="5" t="s">
         <v>100</v>
       </c>
@@ -3916,7 +4065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9">
       <c r="A104" s="5" t="s">
         <v>101</v>
       </c>
@@ -3939,7 +4088,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9">
       <c r="A105" s="5" t="s">
         <v>102</v>
       </c>
@@ -3964,7 +4113,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9">
       <c r="A106" s="5" t="s">
         <v>103</v>
       </c>
@@ -3989,7 +4138,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9">
       <c r="A107" s="5" t="s">
         <v>104</v>
       </c>
@@ -4012,7 +4161,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9">
       <c r="A108" s="5" t="s">
         <v>105</v>
       </c>
@@ -4033,7 +4182,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9">
       <c r="A109" s="5" t="s">
         <v>106</v>
       </c>
@@ -4058,7 +4207,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9">
       <c r="A110" s="5" t="s">
         <v>106</v>
       </c>
@@ -4075,7 +4224,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9">
       <c r="A111" s="5" t="s">
         <v>107</v>
       </c>
@@ -4096,7 +4245,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9">
       <c r="A112" s="5" t="s">
         <v>108</v>
       </c>
@@ -4119,7 +4268,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9">
       <c r="A113" s="5" t="s">
         <v>110</v>
       </c>
@@ -4133,10 +4282,10 @@
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" s="5" t="s">
         <v>111</v>
       </c>
@@ -4150,10 +4299,10 @@
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" s="5" t="s">
         <v>112</v>
       </c>
@@ -4171,10 +4320,10 @@
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116" s="5" t="s">
         <v>113</v>
       </c>
@@ -4192,10 +4341,10 @@
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117" s="5" t="s">
         <v>114</v>
       </c>
@@ -4209,10 +4358,10 @@
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" s="5" t="s">
         <v>115</v>
       </c>
@@ -4230,10 +4379,10 @@
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119" s="5" t="s">
         <v>116</v>
       </c>
@@ -4251,10 +4400,10 @@
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120" s="5" t="s">
         <v>117</v>
       </c>
@@ -4268,10 +4417,10 @@
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121" s="5" t="s">
         <v>118</v>
       </c>
@@ -4285,10 +4434,10 @@
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122" s="5" t="s">
         <v>119</v>
       </c>
@@ -4306,10 +4455,10 @@
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123" s="5" t="s">
         <v>120</v>
       </c>
@@ -4329,10 +4478,10 @@
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" s="5" t="s">
         <v>121</v>
       </c>
@@ -4350,10 +4499,10 @@
       <c r="G124" s="5"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
       <c r="A125" s="5" t="s">
         <v>122</v>
       </c>
@@ -4367,10 +4516,10 @@
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" s="5" t="s">
         <v>123</v>
       </c>
@@ -4388,10 +4537,10 @@
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
       <c r="A127" s="5" t="s">
         <v>124</v>
       </c>
@@ -4405,10 +4554,10 @@
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
       <c r="A128" s="5" t="s">
         <v>125</v>
       </c>
@@ -4422,10 +4571,10 @@
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
       <c r="A129" s="5" t="s">
         <v>126</v>
       </c>
@@ -4439,10 +4588,10 @@
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130" s="5" t="s">
         <v>127</v>
       </c>
@@ -4460,10 +4609,10 @@
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131" s="5" t="s">
         <v>128</v>
       </c>
@@ -4481,10 +4630,10 @@
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132" s="5" t="s">
         <v>129</v>
       </c>
@@ -4502,10 +4651,10 @@
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133" s="5" t="s">
         <v>130</v>
       </c>
@@ -4521,10 +4670,10 @@
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="A134" s="5" t="s">
         <v>131</v>
       </c>
@@ -4538,10 +4687,10 @@
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135" s="5" t="s">
         <v>132</v>
       </c>
@@ -4559,10 +4708,10 @@
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136" s="5" t="s">
         <v>133</v>
       </c>
@@ -4580,16 +4729,16 @@
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137" s="5" t="s">
         <v>134</v>
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="5" t="s">
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
@@ -4599,12 +4748,12 @@
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="5">
@@ -4620,12 +4769,12 @@
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -4637,10 +4786,10 @@
       </c>
       <c r="H139" s="3"/>
       <c r="I139" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
       <c r="A140" s="5" t="s">
         <v>111</v>
       </c>
@@ -4654,12 +4803,12 @@
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
       <c r="A141" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -4671,12 +4820,12 @@
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
       <c r="A142" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -4688,12 +4837,12 @@
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
       <c r="A143" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -4709,12 +4858,12 @@
       <c r="G143" s="5"/>
       <c r="H143" s="3"/>
       <c r="I143" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
       <c r="A144" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="5">
@@ -4730,12 +4879,12 @@
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B145" s="5"/>
       <c r="C145" s="5">
@@ -4751,12 +4900,12 @@
       </c>
       <c r="H145" s="3"/>
       <c r="I145" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B146" s="5"/>
       <c r="C146" s="5">
@@ -4772,12 +4921,12 @@
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
       <c r="A147" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -4789,12 +4938,12 @@
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
       <c r="A148" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
@@ -4806,12 +4955,12 @@
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
       <c r="A149" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B149" s="5"/>
       <c r="C149" s="5">
@@ -4827,12 +4976,12 @@
       </c>
       <c r="H149" s="3"/>
       <c r="I149" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
       <c r="A150" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B150" s="5"/>
       <c r="C150" s="5">
@@ -4848,12 +4997,12 @@
       </c>
       <c r="H150" s="3"/>
       <c r="I150" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
       <c r="A151" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B151" s="5"/>
       <c r="C151" s="5">
@@ -4869,10 +5018,10 @@
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
       <c r="A152" s="5" t="s">
         <v>120</v>
       </c>
@@ -4892,12 +5041,12 @@
       </c>
       <c r="H152" s="3"/>
       <c r="I152" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
       <c r="A153" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
@@ -4909,12 +5058,12 @@
       </c>
       <c r="H153" s="3"/>
       <c r="I153" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
       <c r="A154" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
@@ -4926,12 +5075,12 @@
       </c>
       <c r="H154" s="3"/>
       <c r="I154" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
       <c r="A155" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
@@ -4943,12 +5092,12 @@
       </c>
       <c r="H155" s="3"/>
       <c r="I155" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
       <c r="A156" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B156" s="5"/>
       <c r="C156" s="5">
@@ -4962,16 +5111,16 @@
       </c>
       <c r="H156" s="3"/>
       <c r="I156" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
       <c r="A157" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B157" s="5"/>
       <c r="C157" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
@@ -4981,12 +5130,12 @@
       </c>
       <c r="H157" s="3"/>
       <c r="I157" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
       <c r="A158" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
@@ -4998,12 +5147,12 @@
       </c>
       <c r="H158" s="3"/>
       <c r="I158" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
       <c r="A159" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
@@ -5015,12 +5164,12 @@
       </c>
       <c r="H159" s="3"/>
       <c r="I159" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
       <c r="A160" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B160" s="5"/>
       <c r="C160" s="5">
@@ -5036,12 +5185,12 @@
       </c>
       <c r="H160" s="3"/>
       <c r="I160" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
       <c r="A161" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
@@ -5053,12 +5202,12 @@
       </c>
       <c r="H161" s="3"/>
       <c r="I161" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
       <c r="A162" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B162" s="5"/>
       <c r="C162" s="5">
@@ -5074,12 +5223,12 @@
       </c>
       <c r="H162" s="3"/>
       <c r="I162" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
       <c r="A163" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5">
@@ -5088,57 +5237,57 @@
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G163" s="5">
         <v>112</v>
       </c>
       <c r="H163" s="3"/>
       <c r="I163" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
       <c r="A164" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
       <c r="F164" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G164" s="5">
         <v>116.4</v>
       </c>
       <c r="H164" s="3"/>
       <c r="I164" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
       <c r="A165" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
       <c r="F165" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G165" s="5">
         <v>114.6</v>
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
       <c r="A166" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="5">
@@ -5147,19 +5296,19 @@
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
       <c r="F166" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G166" s="5">
         <v>116.5</v>
       </c>
       <c r="H166" s="3"/>
       <c r="I166" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" s="5" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="5">
@@ -5169,7 +5318,7 @@
         <v>1032</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F167" s="3"/>
       <c r="G167" s="6">
@@ -5177,12 +5326,12 @@
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
       <c r="A168" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B168" s="5"/>
       <c r="C168" s="5">
@@ -5198,12 +5347,12 @@
       </c>
       <c r="H168" s="5"/>
       <c r="I168" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
       <c r="A169" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
@@ -5215,12 +5364,12 @@
       </c>
       <c r="H169" s="5"/>
       <c r="I169" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
       <c r="A170" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
@@ -5232,12 +5381,12 @@
       </c>
       <c r="H170" s="5"/>
       <c r="I170" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
       <c r="A171" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B171" s="5"/>
       <c r="C171" s="5">
@@ -5247,7 +5396,7 @@
         <v>1038</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F171" s="3"/>
       <c r="G171" s="6">
@@ -5255,12 +5404,12 @@
       </c>
       <c r="H171" s="5"/>
       <c r="I171" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
       <c r="A172" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -5272,12 +5421,12 @@
       </c>
       <c r="H172" s="5"/>
       <c r="I172" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
       <c r="A173" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B173" s="5"/>
       <c r="C173" s="5">
@@ -5287,7 +5436,7 @@
         <v>1038</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F173" s="3"/>
       <c r="G173" s="6">
@@ -5295,12 +5444,12 @@
       </c>
       <c r="H173" s="5"/>
       <c r="I173" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
       <c r="A174" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="5">
@@ -5316,12 +5465,12 @@
       </c>
       <c r="H174" s="5"/>
       <c r="I174" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
       <c r="A175" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -5333,12 +5482,12 @@
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
       <c r="A176" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="5">
@@ -5348,7 +5497,7 @@
         <v>1035</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F176" s="3"/>
       <c r="G176" s="6">
@@ -5356,12 +5505,12 @@
       </c>
       <c r="H176" s="5"/>
       <c r="I176" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
+      <c r="A177" s="5" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
@@ -5369,16 +5518,16 @@
       <c r="E177" s="5"/>
       <c r="F177" s="5"/>
       <c r="G177" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
       <c r="A178" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -5386,16 +5535,16 @@
       <c r="E178" s="5"/>
       <c r="F178" s="5"/>
       <c r="G178" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H178" s="5"/>
       <c r="I178" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
       <c r="A179" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
@@ -5405,16 +5554,16 @@
         <v>1190</v>
       </c>
       <c r="G179" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H179" s="5"/>
       <c r="I179" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
       <c r="A180" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
@@ -5422,16 +5571,16 @@
       <c r="E180" s="5"/>
       <c r="F180" s="5"/>
       <c r="G180" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H180" s="5"/>
       <c r="I180" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
+      <c r="A181" s="7" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -5445,12 +5594,12 @@
       </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
       <c r="A182" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B182" s="7"/>
       <c r="C182" s="7">
@@ -5468,12 +5617,12 @@
       </c>
       <c r="H182" s="3"/>
       <c r="I182" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9">
       <c r="A183" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -5487,12 +5636,12 @@
       </c>
       <c r="H183" s="3"/>
       <c r="I183" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
       <c r="A184" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -5506,12 +5655,12 @@
       </c>
       <c r="H184" s="3"/>
       <c r="I184" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9">
       <c r="A185" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -5527,12 +5676,12 @@
       </c>
       <c r="H185" s="3"/>
       <c r="I185" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
       <c r="A186" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -5546,12 +5695,12 @@
       </c>
       <c r="H186" s="3"/>
       <c r="I186" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
+      <c r="A187" s="5" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="B187" s="3"/>
       <c r="C187" s="5">
@@ -5569,12 +5718,12 @@
       </c>
       <c r="H187" s="3"/>
       <c r="I187" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
       <c r="A188" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B188" s="3"/>
       <c r="C188" s="5">
@@ -5592,12 +5741,12 @@
       </c>
       <c r="H188" s="3"/>
       <c r="I188" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9">
       <c r="A189" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B189" s="3"/>
       <c r="C189" s="5">
@@ -5615,12 +5764,12 @@
       </c>
       <c r="H189" s="3"/>
       <c r="I189" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9">
       <c r="A190" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B190" s="3"/>
       <c r="C190" s="5"/>
@@ -5636,12 +5785,12 @@
       </c>
       <c r="H190" s="3"/>
       <c r="I190" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
       <c r="A191" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B191" s="3"/>
       <c r="C191" s="5">
@@ -5659,12 +5808,12 @@
       </c>
       <c r="H191" s="3"/>
       <c r="I191" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9">
       <c r="A192" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B192" s="3"/>
       <c r="C192" s="5"/>
@@ -5680,12 +5829,12 @@
       </c>
       <c r="H192" s="3"/>
       <c r="I192" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9">
       <c r="A193" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B193" s="3"/>
       <c r="C193" s="5"/>
@@ -5701,12 +5850,12 @@
       </c>
       <c r="H193" s="3"/>
       <c r="I193" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9">
       <c r="A194" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B194" s="3"/>
       <c r="C194" s="5"/>
@@ -5722,12 +5871,12 @@
       </c>
       <c r="H194" s="3"/>
       <c r="I194" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9">
       <c r="A195" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B195" s="3"/>
       <c r="C195" s="5"/>
@@ -5743,12 +5892,12 @@
       </c>
       <c r="H195" s="3"/>
       <c r="I195" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9">
       <c r="A196" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B196" s="3"/>
       <c r="C196" s="5"/>
@@ -5764,12 +5913,12 @@
       </c>
       <c r="H196" s="3"/>
       <c r="I196" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9">
       <c r="A197" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B197" s="3"/>
       <c r="C197" s="5">
@@ -5787,7 +5936,7 @@
       </c>
       <c r="H197" s="3"/>
       <c r="I197" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: add reference pdfs
</commit_message>
<xml_diff>
--- a/整理数据.xlsx
+++ b/整理数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yuyouyu\SHU\BMG_Data_SHU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyouyu/WorkSpace/Lab106/Lab_Data/BMG_Data_SHU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303D57CE-C25A-4509-B427-102F2D64A7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6863C4B-22EA-2843-B74D-FF6A36DB3A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{5F0C6EAF-1925-B849-9D8C-419B5710AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1036,7 +1036,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1167,12 +1167,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1180,6 +1174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,7 +1198,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1228,22 +1228,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1262,36 +1246,43 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1606,23 +1597,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1966D2F-1FA9-5C45-AC98-B0EB4D799C65}">
-  <dimension ref="A1:N216"/>
+  <dimension ref="A1:K216"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="38.875" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
-    <col min="7" max="7" width="19.125" customWidth="1"/>
-    <col min="8" max="8" width="17.625" customWidth="1"/>
-    <col min="11" max="11" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>273</v>
       </c>
@@ -1654,20 +1645,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="15">
         <v>7</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="15">
         <v>723</v>
       </c>
       <c r="F2" s="3">
@@ -1676,7 +1667,7 @@
       <c r="G2" s="3">
         <v>1654</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="13" t="s">
         <v>262</v>
       </c>
       <c r="I2" s="3">
@@ -1685,11 +1676,11 @@
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="16" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1708,18 +1699,18 @@
       <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="16" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="15">
         <v>5</v>
       </c>
       <c r="D4" s="3">
@@ -1729,23 +1720,23 @@
       <c r="F4" s="3">
         <v>1115</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="14" t="s">
         <v>259</v>
       </c>
       <c r="H4" s="3">
         <v>86.7</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="13" t="s">
         <v>260</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="17" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1772,11 +1763,11 @@
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="18" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1804,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1832,7 +1823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1860,44 +1851,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="20" customFormat="1">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="19">
         <v>12</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="19">
         <v>641.6</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="19">
         <v>731.9</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="19">
         <v>1168.9000000000001</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="19">
         <v>1872</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26">
+      <c r="H9" s="19"/>
+      <c r="I9" s="19">
         <v>0.1</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="13" t="s">
         <v>269</v>
       </c>
       <c r="D10" s="3">
@@ -1920,14 +1911,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="13" t="s">
         <v>269</v>
       </c>
       <c r="D11" s="3">
@@ -1950,14 +1941,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="13" t="s">
         <v>269</v>
       </c>
       <c r="D12" s="3">
@@ -1980,14 +1971,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="13" t="s">
         <v>269</v>
       </c>
       <c r="D13" s="3">
@@ -2010,7 +2001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2040,364 +2031,356 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+    <row r="15" spans="1:11" s="23" customFormat="1">
+      <c r="B15" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="24">
         <v>22</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="24">
         <v>706</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="24">
         <v>792</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" s="23" customFormat="1">
+      <c r="B16" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="24">
         <v>15</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="24">
         <v>694</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="24">
         <v>787</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-    </row>
-    <row r="17" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="2:10" s="23" customFormat="1">
+      <c r="B17" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="24">
         <v>18</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="24">
         <v>753</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="24">
         <v>797</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-    </row>
-    <row r="18" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="2:10" s="23" customFormat="1">
+      <c r="B18" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="24">
         <v>1.5</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="24">
         <v>657</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="24">
         <v>710</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-    </row>
-    <row r="19" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="2:10" s="23" customFormat="1">
+      <c r="B19" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="24">
         <v>30</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="24">
         <v>683</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="24">
         <v>767</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-    </row>
-    <row r="20" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="2:10" s="23" customFormat="1">
+      <c r="B20" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="24">
         <v>14</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="24">
         <v>719</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="24">
         <v>799</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-    </row>
-    <row r="21" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="2:10" s="23" customFormat="1">
+      <c r="B21" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="24">
         <v>20</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="24">
         <v>655</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="24">
         <v>767</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-    </row>
-    <row r="22" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="2:10" s="23" customFormat="1">
+      <c r="B22" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="24">
         <v>25</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="24">
         <v>683</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="24">
         <v>792</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-    </row>
-    <row r="23" spans="2:14" s="34" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="2:10" s="23" customFormat="1" ht="18">
+      <c r="B23" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="24">
         <v>10</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-    </row>
-    <row r="24" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="2:10" s="23" customFormat="1">
+      <c r="B24" s="24" t="s">
         <v>283</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="24">
         <v>20</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="24">
         <v>755</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="24">
         <v>791</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-    </row>
-    <row r="25" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="2:10" s="23" customFormat="1">
+      <c r="B25" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="24">
         <v>20</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="24">
         <v>714</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="24">
         <v>791</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-    </row>
-    <row r="26" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="2:10" s="23" customFormat="1">
+      <c r="B26" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="24">
         <v>20</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="24">
         <v>694.4</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="24">
         <v>775.9</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-    </row>
-    <row r="27" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+    </row>
+    <row r="27" spans="2:10" s="23" customFormat="1">
+      <c r="B27" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="24">
         <v>16</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="24">
         <v>625</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="24">
         <v>750</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-    </row>
-    <row r="28" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+    </row>
+    <row r="28" spans="2:10" s="23" customFormat="1">
+      <c r="B28" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="24">
         <v>10</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="24">
         <v>625</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="24">
         <v>707</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-    </row>
-    <row r="29" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+    </row>
+    <row r="29" spans="2:10" s="23" customFormat="1">
+      <c r="B29" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="24">
         <v>12</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="24">
         <v>697</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="24">
         <v>758</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-    </row>
-    <row r="30" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+    </row>
+    <row r="30" spans="2:10" s="23" customFormat="1">
+      <c r="B30" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-    </row>
-    <row r="31" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+    </row>
+    <row r="31" spans="2:10" s="23" customFormat="1">
+      <c r="B31" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="24">
         <v>73</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="24">
         <v>705</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="24">
         <v>811</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-    </row>
-    <row r="32" spans="2:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+    </row>
+    <row r="32" spans="2:10" s="23" customFormat="1">
+      <c r="B32" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="24">
         <v>50</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="24">
         <v>625</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="24">
         <v>700</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="B33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1">
       <c r="A34">
         <v>14</v>
       </c>
@@ -2426,9 +2409,9 @@
       <c r="J34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K34" s="25"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>15</v>
       </c>
@@ -2458,7 +2441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>16</v>
       </c>
@@ -2488,7 +2471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>17</v>
       </c>
@@ -2518,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>18</v>
       </c>
@@ -2548,7 +2531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>19</v>
       </c>
@@ -2578,7 +2561,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>20</v>
       </c>
@@ -2608,7 +2591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>21</v>
       </c>
@@ -2638,7 +2621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>22</v>
       </c>
@@ -2670,7 +2653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>23</v>
       </c>
@@ -2702,7 +2685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>24</v>
       </c>
@@ -2734,7 +2717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>25</v>
       </c>
@@ -2766,44 +2749,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="20" customFormat="1">
       <c r="A46">
         <v>26</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="19">
         <v>678</v>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="19">
         <v>710</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="19">
         <v>1161</v>
       </c>
-      <c r="G46" s="26">
+      <c r="G46" s="19">
         <v>1677</v>
       </c>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19">
         <v>7.5</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>27</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="13">
         <v>2</v>
       </c>
       <c r="D47" s="3">
@@ -2826,14 +2809,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>28</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="13">
         <v>2</v>
       </c>
       <c r="D48" s="3">
@@ -2856,46 +2839,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="20" customFormat="1">
       <c r="A49">
         <v>29</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="29">
+      <c r="C49" s="22">
         <v>8</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="19">
         <v>660.6</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="19">
         <v>715.2</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F49" s="19">
         <v>1153.7</v>
       </c>
-      <c r="G49" s="26">
+      <c r="G49" s="19">
         <v>1469</v>
       </c>
-      <c r="H49" s="26">
+      <c r="H49" s="19">
         <v>257.5</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="19">
         <v>0.11</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>30</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="21">
+      <c r="C50" s="15">
         <v>8</v>
       </c>
       <c r="D50" s="3">
@@ -2920,14 +2903,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="21">
+      <c r="C51" s="15">
         <v>8</v>
       </c>
       <c r="D51" s="3">
@@ -2952,14 +2935,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>32</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="21">
+      <c r="C52" s="15">
         <v>8</v>
       </c>
       <c r="D52" s="3">
@@ -2984,7 +2967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>33</v>
       </c>
@@ -3012,7 +2995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>34</v>
       </c>
@@ -3040,7 +3023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>35</v>
       </c>
@@ -3068,7 +3051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>36</v>
       </c>
@@ -3094,7 +3077,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>37</v>
       </c>
@@ -3124,7 +3107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>38</v>
       </c>
@@ -3154,7 +3137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>39</v>
       </c>
@@ -3180,7 +3163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>40</v>
       </c>
@@ -3206,7 +3189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>41</v>
       </c>
@@ -3230,7 +3213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>42</v>
       </c>
@@ -3254,7 +3237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>43</v>
       </c>
@@ -3286,7 +3269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>44</v>
       </c>
@@ -3314,7 +3297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>45</v>
       </c>
@@ -3342,7 +3325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>46</v>
       </c>
@@ -3370,7 +3353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>47</v>
       </c>
@@ -3398,7 +3381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>48</v>
       </c>
@@ -3424,7 +3407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>49</v>
       </c>
@@ -3454,7 +3437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>50</v>
       </c>
@@ -3484,7 +3467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>51</v>
       </c>
@@ -3514,7 +3497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>52</v>
       </c>
@@ -3544,7 +3527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>53</v>
       </c>
@@ -3574,35 +3557,35 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="74" spans="1:10" s="26" customFormat="1">
+      <c r="A74" s="26">
         <v>54</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="C74" s="14">
+      <c r="C74" s="28">
         <v>73</v>
       </c>
-      <c r="D74" s="14">
+      <c r="D74" s="28">
         <v>705</v>
       </c>
-      <c r="E74" s="14">
+      <c r="E74" s="28">
         <v>811</v>
       </c>
-      <c r="F74" s="14">
+      <c r="F74" s="28">
         <v>1103</v>
       </c>
-      <c r="G74" s="14"/>
-      <c r="H74" s="15">
+      <c r="G74" s="28"/>
+      <c r="H74" s="29">
         <v>96.3</v>
       </c>
-      <c r="I74" s="16"/>
-      <c r="J74" s="17" t="s">
+      <c r="I74" s="30"/>
+      <c r="J74" s="31" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>55</v>
       </c>
@@ -3630,7 +3613,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>56</v>
       </c>
@@ -3660,7 +3643,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>57</v>
       </c>
@@ -3688,7 +3671,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>58</v>
       </c>
@@ -3714,7 +3697,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>59</v>
       </c>
@@ -3740,7 +3723,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>60</v>
       </c>
@@ -3766,7 +3749,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>61</v>
       </c>
@@ -3792,7 +3775,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>62</v>
       </c>
@@ -3818,7 +3801,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>63</v>
       </c>
@@ -3844,7 +3827,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>64</v>
       </c>
@@ -3870,7 +3853,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>65</v>
       </c>
@@ -3900,7 +3883,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>66</v>
       </c>
@@ -3926,7 +3909,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>67</v>
       </c>
@@ -3954,7 +3937,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>68</v>
       </c>
@@ -3984,7 +3967,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>69</v>
       </c>
@@ -4014,7 +3997,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>70</v>
       </c>
@@ -4040,7 +4023,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>71</v>
       </c>
@@ -4066,7 +4049,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>72</v>
       </c>
@@ -4096,7 +4079,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>73</v>
       </c>
@@ -4126,7 +4109,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>74</v>
       </c>
@@ -4154,7 +4137,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>75</v>
       </c>
@@ -4184,7 +4167,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>76</v>
       </c>
@@ -4212,7 +4195,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="1" customFormat="1">
       <c r="A97">
         <v>77</v>
       </c>
@@ -4238,7 +4221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="A98">
         <v>78</v>
       </c>
@@ -4264,7 +4247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99">
         <v>79</v>
       </c>
@@ -4290,7 +4273,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="A100">
         <v>80</v>
       </c>
@@ -4312,7 +4295,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="A101">
         <v>81</v>
       </c>
@@ -4336,7 +4319,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="A102">
         <v>82</v>
       </c>
@@ -4358,7 +4341,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11">
       <c r="A103">
         <v>83</v>
       </c>
@@ -4380,7 +4363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11">
       <c r="A104">
         <v>84</v>
       </c>
@@ -4404,7 +4387,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11">
       <c r="A105">
         <v>85</v>
       </c>
@@ -4432,7 +4415,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11">
       <c r="A106">
         <v>86</v>
       </c>
@@ -4458,7 +4441,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11">
       <c r="A107">
         <v>87</v>
       </c>
@@ -4484,7 +4467,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11">
       <c r="A108">
         <v>88</v>
       </c>
@@ -4511,7 +4494,7 @@
       </c>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11">
       <c r="A109">
         <v>89</v>
       </c>
@@ -4537,7 +4520,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11">
       <c r="A110">
         <v>90</v>
       </c>
@@ -4563,7 +4546,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11">
       <c r="A111">
         <v>91</v>
       </c>
@@ -4587,7 +4570,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11">
       <c r="A112">
         <v>92</v>
       </c>
@@ -4613,7 +4596,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>93</v>
       </c>
@@ -4637,7 +4620,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>94</v>
       </c>
@@ -4663,7 +4646,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>95</v>
       </c>
@@ -4687,7 +4670,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>96</v>
       </c>
@@ -4715,7 +4698,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>97</v>
       </c>
@@ -4743,7 +4726,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>98</v>
       </c>
@@ -4769,7 +4752,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>99</v>
       </c>
@@ -4795,7 +4778,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>100</v>
       </c>
@@ -4821,7 +4804,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121">
         <v>101</v>
       </c>
@@ -4841,7 +4824,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>102</v>
       </c>
@@ -4867,7 +4850,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>103</v>
       </c>
@@ -4893,7 +4876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124">
         <v>104</v>
       </c>
@@ -4921,7 +4904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>105</v>
       </c>
@@ -4949,7 +4932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>106</v>
       </c>
@@ -4975,7 +4958,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>107</v>
       </c>
@@ -4999,7 +4982,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>108</v>
       </c>
@@ -5027,7 +5010,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129">
         <v>109</v>
       </c>
@@ -5047,7 +5030,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130">
         <v>110</v>
       </c>
@@ -5071,7 +5054,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131">
         <v>111</v>
       </c>
@@ -5097,7 +5080,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132">
         <v>112</v>
       </c>
@@ -5117,7 +5100,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133">
         <v>113</v>
       </c>
@@ -5137,7 +5120,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134">
         <v>114</v>
       </c>
@@ -5161,7 +5144,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135">
         <v>115</v>
       </c>
@@ -5185,7 +5168,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136">
         <v>116</v>
       </c>
@@ -5205,7 +5188,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137">
         <v>117</v>
       </c>
@@ -5229,7 +5212,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138">
         <v>118</v>
       </c>
@@ -5253,7 +5236,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139">
         <v>119</v>
       </c>
@@ -5273,7 +5256,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140">
         <v>120</v>
       </c>
@@ -5293,7 +5276,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141">
         <v>121</v>
       </c>
@@ -5317,7 +5300,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142">
         <v>122</v>
       </c>
@@ -5343,7 +5326,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143">
         <v>123</v>
       </c>
@@ -5367,7 +5350,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144">
         <v>124</v>
       </c>
@@ -5387,7 +5370,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145">
         <v>125</v>
       </c>
@@ -5411,7 +5394,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146">
         <v>126</v>
       </c>
@@ -5431,7 +5414,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147">
         <v>127</v>
       </c>
@@ -5451,7 +5434,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148">
         <v>128</v>
       </c>
@@ -5471,7 +5454,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149">
         <v>129</v>
       </c>
@@ -5495,7 +5478,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150">
         <v>130</v>
       </c>
@@ -5519,7 +5502,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151">
         <v>131</v>
       </c>
@@ -5543,7 +5526,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152">
         <v>132</v>
       </c>
@@ -5565,7 +5548,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153">
         <v>133</v>
       </c>
@@ -5585,7 +5568,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154">
         <v>134</v>
       </c>
@@ -5609,7 +5592,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155">
         <v>135</v>
       </c>
@@ -5633,7 +5616,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156">
         <v>136</v>
       </c>
@@ -5655,7 +5638,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157">
         <v>137</v>
       </c>
@@ -5679,7 +5662,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158">
         <v>138</v>
       </c>
@@ -5699,7 +5682,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159">
         <v>139</v>
       </c>
@@ -5719,7 +5702,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160">
         <v>140</v>
       </c>
@@ -5739,7 +5722,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161">
         <v>141</v>
       </c>
@@ -5759,7 +5742,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162">
         <v>142</v>
       </c>
@@ -5783,7 +5766,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163">
         <v>143</v>
       </c>
@@ -5807,7 +5790,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164">
         <v>144</v>
       </c>
@@ -5831,7 +5814,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165">
         <v>145</v>
       </c>
@@ -5855,7 +5838,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166">
         <v>146</v>
       </c>
@@ -5875,7 +5858,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167">
         <v>147</v>
       </c>
@@ -5895,7 +5878,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168">
         <v>148</v>
       </c>
@@ -5919,7 +5902,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169">
         <v>149</v>
       </c>
@@ -5943,7 +5926,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170">
         <v>150</v>
       </c>
@@ -5967,7 +5950,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171">
         <v>151</v>
       </c>
@@ -5993,7 +5976,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172">
         <v>152</v>
       </c>
@@ -6013,7 +5996,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173">
         <v>153</v>
       </c>
@@ -6033,7 +6016,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174">
         <v>154</v>
       </c>
@@ -6053,7 +6036,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175">
         <v>155</v>
       </c>
@@ -6075,7 +6058,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176">
         <v>156</v>
       </c>
@@ -6097,7 +6080,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177">
         <v>157</v>
       </c>
@@ -6117,7 +6100,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178">
         <v>158</v>
       </c>
@@ -6137,7 +6120,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179">
         <v>159</v>
       </c>
@@ -6161,7 +6144,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180">
         <v>160</v>
       </c>
@@ -6181,7 +6164,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181">
         <v>161</v>
       </c>
@@ -6205,7 +6188,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182">
         <v>162</v>
       </c>
@@ -6229,7 +6212,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183">
         <v>163</v>
       </c>
@@ -6251,7 +6234,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184">
         <v>164</v>
       </c>
@@ -6273,7 +6256,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185">
         <v>165</v>
       </c>
@@ -6297,7 +6280,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186">
         <v>166</v>
       </c>
@@ -6323,7 +6306,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187">
         <v>167</v>
       </c>
@@ -6347,7 +6330,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188">
         <v>168</v>
       </c>
@@ -6367,7 +6350,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189">
         <v>169</v>
       </c>
@@ -6387,7 +6370,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190">
         <v>170</v>
       </c>
@@ -6413,7 +6396,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191">
         <v>171</v>
       </c>
@@ -6433,7 +6416,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192">
         <v>172</v>
       </c>
@@ -6459,7 +6442,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193">
         <v>173</v>
       </c>
@@ -6483,7 +6466,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194">
         <v>174</v>
       </c>
@@ -6503,7 +6486,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195">
         <v>175</v>
       </c>
@@ -6529,7 +6512,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196">
         <v>176</v>
       </c>
@@ -6549,7 +6532,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197">
         <v>177</v>
       </c>
@@ -6569,7 +6552,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198">
         <v>178</v>
       </c>
@@ -6591,7 +6574,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199">
         <v>179</v>
       </c>
@@ -6611,7 +6594,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200">
         <v>180</v>
       </c>
@@ -6633,7 +6616,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201">
         <v>181</v>
       </c>
@@ -6659,7 +6642,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202">
         <v>182</v>
       </c>
@@ -6681,7 +6664,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203">
         <v>183</v>
       </c>
@@ -6703,7 +6686,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204">
         <v>184</v>
       </c>
@@ -6727,7 +6710,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205">
         <v>185</v>
       </c>
@@ -6749,7 +6732,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206">
         <v>186</v>
       </c>
@@ -6775,7 +6758,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207">
         <v>187</v>
       </c>
@@ -6801,7 +6784,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208">
         <v>188</v>
       </c>
@@ -6827,7 +6810,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209">
         <v>189</v>
       </c>
@@ -6851,7 +6834,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210">
         <v>190</v>
       </c>
@@ -6877,7 +6860,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211">
         <v>191</v>
       </c>
@@ -6901,7 +6884,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212">
         <v>192</v>
       </c>
@@ -6925,7 +6908,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213">
         <v>193</v>
       </c>
@@ -6949,7 +6932,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214">
         <v>194</v>
       </c>
@@ -6973,7 +6956,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215">
         <v>195</v>
       </c>
@@ -6997,7 +6980,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216">
         <v>196</v>
       </c>

</xml_diff>